<commit_message>
Solved issue of logger in parallel testing.
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/Kisan.NetTestData.xlsx
+++ b/src/main/resources/testData/Kisan.NetTestData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="LoginData" sheetId="1" r:id="rId3"/>
@@ -28,79 +28,79 @@
     <t>Password</t>
   </si>
   <si>
+    <t>runMode</t>
+  </si>
+  <si>
     <t>ChannelName</t>
   </si>
   <si>
+    <t>exh_1003@mailinator.com</t>
+  </si>
+  <si>
     <t>AboutChannel</t>
   </si>
   <si>
-    <t>runMode</t>
-  </si>
-  <si>
     <t>HexColor</t>
   </si>
   <si>
     <t>Message</t>
   </si>
   <si>
-    <t>exh_1003@mailinator.com</t>
-  </si>
-  <si>
     <t>chan@kisan18</t>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
+    <t>Edited Channel</t>
+  </si>
+  <si>
     <t>Channel 1003</t>
   </si>
   <si>
-    <t>Edited Channel</t>
+    <t>Description added by script</t>
   </si>
   <si>
     <t>Hey followers, Automation in progress</t>
   </si>
   <si>
-    <t>Description added by script</t>
-  </si>
-  <si>
     <t>#551d84</t>
   </si>
   <si>
+    <t>Namaskar</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>HelpText</t>
+  </si>
+  <si>
     <t>Channel 1010</t>
   </si>
   <si>
     <t>Hey, This is automated message.</t>
   </si>
   <si>
-    <t>Namaskar</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>HelpText</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
     <t>Namaskar!</t>
   </si>
   <si>
+    <t>Web App Version 6.7</t>
+  </si>
+  <si>
+    <t>We would be happy to help you.</t>
+  </si>
+  <si>
     <t>app@kisan.com</t>
   </si>
   <si>
     <t>020-3025-2020</t>
-  </si>
-  <si>
-    <t>We would be happy to help you.</t>
-  </si>
-  <si>
-    <t>Web App Version 6.7</t>
   </si>
   <si>
     <t>UserName</t>
@@ -209,54 +209,57 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="4" max="4" width="11.0"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -266,12 +269,12 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -286,7 +289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -303,15 +306,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -329,7 +332,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -346,21 +349,73 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -372,19 +427,16 @@
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -401,27 +453,27 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
@@ -432,57 +484,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -502,21 +505,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -525,10 +528,10 @@
         <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>
@@ -540,7 +543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -557,24 +560,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -583,14 +586,14 @@
         <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
@@ -601,7 +604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -621,12 +624,12 @@
         <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -644,7 +647,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -661,18 +664,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -693,7 +696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -710,18 +713,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -738,7 +741,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>

</xml_diff>